<commit_message>
Added rcalc and main run parameters.
</commit_message>
<xml_diff>
--- a/abm/input/pak/Scenarios of vaccine roll out 2.xlsx
+++ b/abm/input/pak/Scenarios of vaccine roll out 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\ABM\CovidABM\abm\input\pak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66200F5-7D33-4CA3-8059-DE3EF217AE87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7117A1-CCA3-4C91-8C8E-766AAF912117}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D42993B8-8161-4F81-AAC1-91E7DB8E02F9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D42993B8-8161-4F81-AAC1-91E7DB8E02F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Vers 1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="138">
   <si>
     <t>Rural (World Bank 2020)</t>
   </si>
@@ -24062,7 +24062,7 @@
   <dimension ref="A1:X35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24132,6 +24132,9 @@
       <c r="J3" t="s">
         <v>137</v>
       </c>
+      <c r="K3" t="s">
+        <v>133</v>
+      </c>
       <c r="O3" t="s">
         <v>109</v>
       </c>
@@ -24188,6 +24191,10 @@
         <f>X4</f>
         <v>36</v>
       </c>
+      <c r="K4" t="str">
+        <f>V4</f>
+        <v>9</v>
+      </c>
       <c r="N4" t="s">
         <v>5</v>
       </c>
@@ -24251,6 +24258,10 @@
         <f t="shared" ref="J5:J12" si="0">X5</f>
         <v>265</v>
       </c>
+      <c r="K5" t="str">
+        <f t="shared" ref="K5:K12" si="1">V5</f>
+        <v>66</v>
+      </c>
       <c r="O5" t="s">
         <v>23</v>
       </c>
@@ -24263,19 +24274,19 @@
         <v>40724136.768097505</v>
       </c>
       <c r="S5" s="119">
-        <f t="shared" ref="S5:S12" si="1">P5/(1+2*$Q$14/(1-$Q$14))</f>
+        <f t="shared" ref="S5:S12" si="2">P5/(1+2*$Q$14/(1-$Q$14))</f>
         <v>5934532.4572778633</v>
       </c>
       <c r="T5" s="119">
-        <f t="shared" ref="T5:T12" si="2">(P5-S5)/2</f>
+        <f t="shared" ref="T5:T12" si="3">(P5-S5)/2</f>
         <v>17803597.371833589</v>
       </c>
       <c r="V5" t="str">
-        <f t="shared" ref="V5:V12" si="3">FIXED(S5*$Q$15/$Q$16,0)</f>
+        <f t="shared" ref="V5:V12" si="4">FIXED(S5*$Q$15/$Q$16,0)</f>
         <v>66</v>
       </c>
       <c r="W5" t="str">
-        <f t="shared" ref="W5:W12" si="4">FIXED(T5*$Q$15/$Q$16,0)</f>
+        <f t="shared" ref="W5:W12" si="5">FIXED(T5*$Q$15/$Q$16,0)</f>
         <v>199</v>
       </c>
       <c r="X5">
@@ -24312,6 +24323,10 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
       <c r="O6" s="27" t="s">
         <v>21</v>
       </c>
@@ -24324,20 +24339,20 @@
         <v>11602801.340801064</v>
       </c>
       <c r="S6" s="119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>675959.32335105818</v>
       </c>
       <c r="T6" s="119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2027877.9700531745</v>
       </c>
       <c r="U6" s="27"/>
       <c r="V6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="W6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="X6">
@@ -24360,7 +24375,7 @@
         <v>87</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7:E12" si="5">A7/$I$5</f>
+        <f t="shared" ref="E7:E12" si="6">A7/$I$5</f>
         <v>0.3282937365010799</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -24374,6 +24389,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O7" s="1" t="s">
         <v>9</v>
       </c>
@@ -24386,20 +24405,20 @@
         <v>14834500.179531109</v>
       </c>
       <c r="S7" s="119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T7" s="119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U7" s="1"/>
       <c r="V7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X7">
@@ -24422,7 +24441,7 @@
         <v>5</v>
       </c>
       <c r="E8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.9438444924406047E-2</v>
       </c>
       <c r="G8" t="s">
@@ -24439,6 +24458,10 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
+      <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
       <c r="N8" t="s">
         <v>6</v>
       </c>
@@ -24454,19 +24477,19 @@
         <v>7571946.6732167117</v>
       </c>
       <c r="S8" s="119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>943056.19661409035</v>
       </c>
       <c r="T8" s="119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2829168.5898422711</v>
       </c>
       <c r="V8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="W8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="X8">
@@ -24489,7 +24512,7 @@
         <v>57</v>
       </c>
       <c r="E9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.21382289416846653</v>
       </c>
       <c r="H9" t="s">
@@ -24503,6 +24526,10 @@
         <f t="shared" si="0"/>
         <v>306</v>
       </c>
+      <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
       <c r="O9" t="s">
         <v>23</v>
       </c>
@@ -24515,19 +24542,19 @@
         <v>69341097.740274146</v>
       </c>
       <c r="S9" s="119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6853705.6357060587</v>
       </c>
       <c r="T9" s="119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20561116.907118175</v>
       </c>
       <c r="V9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>76</v>
       </c>
       <c r="W9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>229</v>
       </c>
       <c r="X9">
@@ -24550,7 +24577,7 @@
         <v>42</v>
       </c>
       <c r="E10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.15766738660907129</v>
       </c>
       <c r="H10" s="27" t="s">
@@ -24564,6 +24591,10 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
+      <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
       <c r="O10" s="27" t="s">
         <v>21</v>
       </c>
@@ -24576,20 +24607,20 @@
         <v>19756121.201904517</v>
       </c>
       <c r="S10" s="119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>780655.63838608656</v>
       </c>
       <c r="T10" s="119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2341966.9151582597</v>
       </c>
       <c r="U10" s="27"/>
       <c r="V10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="W10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="X10">
@@ -24612,7 +24643,7 @@
         <v>38</v>
       </c>
       <c r="E11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.14254859611231102</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -24626,6 +24657,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="O11" s="1" t="s">
         <v>9</v>
       </c>
@@ -24638,20 +24673,20 @@
         <v>25258743.548931349</v>
       </c>
       <c r="S11" s="119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T11" s="119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U11" s="1"/>
       <c r="V11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X11">
@@ -24691,6 +24726,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="N12" t="s">
         <v>54</v>
       </c>
@@ -24702,19 +24741,19 @@
         <v>30526483.028257299</v>
       </c>
       <c r="S12" s="119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T12" s="119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X12">
@@ -24737,7 +24776,7 @@
         <v>9</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="E13:E15" si="6">A13/$I$4</f>
+        <f t="shared" ref="E13:E15" si="7">A13/$I$4</f>
         <v>0.25862068965517243</v>
       </c>
       <c r="P13" s="48"/>
@@ -24757,7 +24796,7 @@
         <v>11</v>
       </c>
       <c r="E14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.31034482758620691</v>
       </c>
       <c r="P14" t="s">
@@ -24786,7 +24825,7 @@
         <v>3</v>
       </c>
       <c r="E15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.6206896551724144E-2</v>
       </c>
       <c r="P15" t="s">
@@ -24838,7 +24877,7 @@
         <v>5</v>
       </c>
       <c r="E17">
-        <f t="shared" ref="E16:E18" si="7">A17/$I$5</f>
+        <f t="shared" ref="E16:E18" si="8">A17/$I$5</f>
         <v>1.7278617710583154E-2</v>
       </c>
     </row>
@@ -24857,7 +24896,7 @@
         <v>2</v>
       </c>
       <c r="E18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8.6393088552915772E-3</v>
       </c>
       <c r="Q18" s="38"/>
@@ -24964,7 +25003,7 @@
         <v>90</v>
       </c>
       <c r="E24">
-        <f t="shared" ref="E24:E28" si="8">A24/$I$9</f>
+        <f t="shared" ref="E24:E28" si="9">A24/$I$9</f>
         <v>0.29545454545454547</v>
       </c>
     </row>
@@ -24983,7 +25022,7 @@
         <v>7</v>
       </c>
       <c r="E25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.1390374331550801E-2</v>
       </c>
     </row>
@@ -25002,7 +25041,7 @@
         <v>69</v>
       </c>
       <c r="E26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.22459893048128343</v>
       </c>
     </row>
@@ -25021,7 +25060,7 @@
         <v>47</v>
       </c>
       <c r="E27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.15508021390374332</v>
       </c>
     </row>
@@ -25040,7 +25079,7 @@
         <v>44</v>
       </c>
       <c r="E28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.14438502673796791</v>
       </c>
     </row>
@@ -25078,7 +25117,7 @@
         <v>10</v>
       </c>
       <c r="E30">
-        <f t="shared" ref="E30:E32" si="9">A30/$I$8</f>
+        <f t="shared" ref="E30:E32" si="10">A30/$I$8</f>
         <v>0.24778761061946902</v>
       </c>
     </row>
@@ -25097,7 +25136,7 @@
         <v>13</v>
       </c>
       <c r="E31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.30088495575221241</v>
       </c>
     </row>
@@ -25116,7 +25155,7 @@
         <v>4</v>
       </c>
       <c r="E32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.8495575221238937E-2</v>
       </c>
     </row>
@@ -25135,7 +25174,7 @@
         <v>10</v>
       </c>
       <c r="E33">
-        <f t="shared" ref="E33" si="10">A33/$I$9</f>
+        <f t="shared" ref="E33" si="11">A33/$I$9</f>
         <v>3.2085561497326207E-2</v>
       </c>
     </row>
@@ -25154,7 +25193,7 @@
         <v>6</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E35" si="11">A34/$I$9</f>
+        <f t="shared" ref="E34:E35" si="12">A34/$I$9</f>
         <v>2.0053475935828877E-2</v>
       </c>
     </row>
@@ -25173,7 +25212,7 @@
         <v>3</v>
       </c>
       <c r="E35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.06951871657754E-2</v>
       </c>
     </row>
@@ -25190,10 +25229,13 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="C1" t="s">

</xml_diff>